<commit_message>
Finished performer in ReFramework
</commit_message>
<xml_diff>
--- a/Payslip process/Config/Config.xlsx
+++ b/Payslip process/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\premal\Google Drive\QAC projects\HR automation\automation\HR-Payroll-automation\Payslip process\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BFCD8F-3386-4403-9C64-0185CAA0194C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBFE39C-EAC3-4148-B6FD-22862B3E9C04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Sheet1</t>
+  </si>
+  <si>
+    <t>payslip_template_employees.xlsx</t>
+  </si>
+  <si>
+    <t>Payslip template</t>
   </si>
 </sst>
 </file>
@@ -511,7 +517,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -616,7 +622,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Got performer working in payslip process need to fix issue with hourly rate not showing up
</commit_message>
<xml_diff>
--- a/Payslip process/Config/Config.xlsx
+++ b/Payslip process/Config/Config.xlsx
@@ -8,21 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\premal\Google Drive\QAC projects\HR automation\automation\HR-Payroll-automation\Payslip process\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBFE39C-EAC3-4148-B6FD-22862B3E9C04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AEEA3A-BE2E-4B96-8C66-1F75414C89D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -138,6 +148,27 @@
   </si>
   <si>
     <t>Payslip template</t>
+  </si>
+  <si>
+    <t>Payslip payroll template</t>
+  </si>
+  <si>
+    <t>C:\\Users\\premal\\Google Drive\\QAC projects\\HR automation\\automation\\HR-Payroll-automation\\Payslip process\\DataBases\\payslip_template_employees.xlsx</t>
+  </si>
+  <si>
+    <t>Payslip save location</t>
+  </si>
+  <si>
+    <t>C:\\Users\\premal\\Google Drive\\QAC projects\\HR automation\\automation\\HR-Payroll-automation\\Payslip process\\Payslips\\</t>
+  </si>
+  <si>
+    <t>URL DKK</t>
+  </si>
+  <si>
+    <t>https://www.xe.com/currencyconverter/convert/?Amount=1&amp;From=GBP&amp;To=DKK</t>
+  </si>
+  <si>
+    <t>Website to scrape DKK conversion rate</t>
   </si>
 </sst>
 </file>
@@ -517,7 +548,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -630,9 +661,33 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>